<commit_message>
Actualizacion de verificacion origen - destino
</commit_message>
<xml_diff>
--- a/Plantilla Tarifario.xlsx
+++ b/Plantilla Tarifario.xlsx
@@ -5,25 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfgalvis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfgalvis\Documents\Proyecto_Tarificador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73888F3D-16CE-4A95-A89D-E4F3EF7C3F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EEF947E-F8F9-4B42-A9F3-39BA0EC0F7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarifario" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarifario!$B$3:$B$3</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Destino</t>
   </si>
@@ -35,6 +32,12 @@
   </si>
   <si>
     <t>Tarifa Recomentada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogota </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cali </t>
   </si>
 </sst>
 </file>
@@ -512,54 +515,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F4"/>
+  <dimension ref="B1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="7"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>